<commit_message>
Added categoryId to excel
</commit_message>
<xml_diff>
--- a/assets/excel_example.xlsx
+++ b/assets/excel_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">Артикул</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Наличие (+ або -)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Категория №</t>
   </si>
   <si>
     <t xml:space="preserve">Бренд</t>
@@ -377,38 +380,39 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BE65536"/>
+  <dimension ref="A1:BF8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.0971659919028"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="24" min="14" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="30" min="26" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="34" min="33" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="41" min="36" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="53" min="43" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="57" min="55" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="58" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7773279352227"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="31" min="27" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="42" min="37" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="54" min="44" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="58" min="56" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1025" min="59" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,7 +440,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -582,11 +586,13 @@
       </c>
       <c r="BE1" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="48.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Categories list can be changed in Excel. Added CompanyName input
</commit_message>
<xml_diff>
--- a/assets/excel_example.xlsx
+++ b/assets/excel_example.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Товары" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Категории" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t xml:space="preserve">Артикул</t>
   </si>
@@ -194,6 +195,132 @@
   </si>
   <si>
     <t xml:space="preserve">Разъем для наушников</t>
+  </si>
+  <si>
+    <t xml:space="preserve">№</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Категория</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мобильные телефоны</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аксессуары для мобильных телефонов и смартфонов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Компьютеры и ноутбуки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Медиаплееры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Автопринадлежности</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Красота, здоровье, уход</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Камеры заднего вида</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Электроника</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Игрушки для детей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спорт, Здоровье, Туризм</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Всё для ремонта, инструменты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV Shop товары</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кошельки и клатчи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гаджеты и подарки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Метеостанции и барометры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Уход и хранение одежды и обуви</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Садовый инвентарь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Электрические проточные водонагреватели</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шведские стенки и турники</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шланги</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ночники</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аксессуары для дверей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кофеварки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рюкзаки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Уличное освещение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наушники</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чехлы для мобильных телефонов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Акустические системы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мыши</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ручные/Автомобильные пылесосы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Планшеты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зарядные устройства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Термосы и бутылки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FM-трансмиттеры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Видеорегистраторы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дневные ходовые огни</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Блоки питания для ноутбуков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Машинки для стрижки и триммеры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Эпиляторы и женские электробритвы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Держатели</t>
   </si>
 </sst>
 </file>
@@ -203,7 +330,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -233,6 +360,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -289,7 +422,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,6 +433,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -377,41 +522,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BF8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7773279352227"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.7408906882591"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="31" min="27" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="31" min="27" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="42" min="37" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="54" min="44" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="58" min="56" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="42" min="37" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="54" min="44" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="58" min="56" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="59" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -602,4 +746,361 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04048582995952"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.2874493927126"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added State and OldPrice for goods
</commit_message>
<xml_diff>
--- a/assets/excel_example.xlsx
+++ b/assets/excel_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Товары" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t xml:space="preserve">Артикул</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t xml:space="preserve">Описание</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Состояние товара</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Старая цена</t>
   </si>
   <si>
     <t xml:space="preserve">Розничная цена</t>
@@ -524,42 +530,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BF8"/>
+  <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.7408906882591"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="31" min="27" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="42" min="37" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="54" min="44" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="58" min="56" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="1025" min="59" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.0607287449393"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="27" min="17" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="33" min="29" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="37" min="36" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="44" min="39" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="56" min="46" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="60" min="58" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="61" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,10 +593,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -733,6 +739,12 @@
       </c>
       <c r="BF1" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="48.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -755,23 +767,22 @@
   </sheetPr>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04048582995952"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.2874493927126"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,7 +806,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,7 +814,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -811,7 +822,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,7 +846,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,7 +854,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +862,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +870,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,7 +878,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,7 +886,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,7 +894,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,7 +902,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,7 +910,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,7 +918,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,7 +926,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,7 +934,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,7 +942,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,7 +950,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +958,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,7 +966,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,7 +974,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,7 +982,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,7 +990,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,7 +998,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,7 +1006,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,7 +1014,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1022,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,7 +1030,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,7 +1038,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,7 +1054,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,7 +1062,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1059,7 +1070,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,7 +1078,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1086,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,7 +1094,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,7 +1102,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>